<commit_message>
rename Ehexcel2 -> Ehexcel
</commit_message>
<xml_diff>
--- a/Ehexcel2/testdata/output.xlsx
+++ b/Ehexcel2/testdata/output.xlsx
@@ -406,7 +406,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -417,43 +417,29 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.5"/>
   </cols>
   <sheetData>
     <row r="1"/>
     <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5">
-      <c r="A5" s="1" t="s"/>
-      <c r="B5" s="1" t="s"/>
-      <c r="C5" s="1" t="s"/>
-      <c r="D5" s="1" t="s"/>
-      <c r="E5" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s"/>
-      <c r="B6" s="1" t="s"/>
-      <c r="C6" s="1" t="s"/>
-      <c r="D6" s="1" t="s"/>
-      <c r="E6" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>